<commit_message>
adding new facebook domains
</commit_message>
<xml_diff>
--- a/blocklist work in process.xlsx
+++ b/blocklist work in process.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brian\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brian\Documents\Git Projects\Ad List\adlist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B08411-332A-4253-A5B0-B922F024C998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED335038-2F96-436D-AEFD-C733D554C0FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="28800" windowHeight="15370" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exact List" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5160" uniqueCount="1321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5400" uniqueCount="1441">
   <si>
     <t>api-v3.tinypass.com</t>
   </si>
@@ -3985,6 +3985,366 @@
   </si>
   <si>
     <t>twitterstat.us</t>
+  </si>
+  <si>
+    <t>el-gr.facebook.com</t>
+  </si>
+  <si>
+    <t>es-la.facebook.com</t>
+  </si>
+  <si>
+    <t>tl-ph.facebook.com</t>
+  </si>
+  <si>
+    <t>act.facebook.com</t>
+  </si>
+  <si>
+    <t>es.facebook.com</t>
+  </si>
+  <si>
+    <t>graph.facebook.com</t>
+  </si>
+  <si>
+    <t>developers.facebook.com</t>
+  </si>
+  <si>
+    <t>zh-cn.connect.facebook.com</t>
+  </si>
+  <si>
+    <t>fi-fi.facebook.com</t>
+  </si>
+  <si>
+    <t>code.facebook.com</t>
+  </si>
+  <si>
+    <t>ns2.facebook.com</t>
+  </si>
+  <si>
+    <t>tr.facebook.com</t>
+  </si>
+  <si>
+    <t>th-th.facebook.com</t>
+  </si>
+  <si>
+    <t>dns.facebook.com</t>
+  </si>
+  <si>
+    <t>vi-vn.connect.facebook.com</t>
+  </si>
+  <si>
+    <t>csf.facebook.com</t>
+  </si>
+  <si>
+    <t>intern.facebook.com</t>
+  </si>
+  <si>
+    <t>x.facebook.com</t>
+  </si>
+  <si>
+    <t>bc.facebook.com</t>
+  </si>
+  <si>
+    <t>ar-ar.facebook.com</t>
+  </si>
+  <si>
+    <t>es-es.fbjs.facebook.com</t>
+  </si>
+  <si>
+    <t>ja-jp.facebook.com</t>
+  </si>
+  <si>
+    <t>id-id.facebook.com</t>
+  </si>
+  <si>
+    <t>ntp.facebook.com</t>
+  </si>
+  <si>
+    <t>static.ak.connect.facebook.com</t>
+  </si>
+  <si>
+    <t>nic.facebook.com</t>
+  </si>
+  <si>
+    <t>w.facebook.com</t>
+  </si>
+  <si>
+    <t>zh-tw.facebook.com</t>
+  </si>
+  <si>
+    <t>o.facebook.com</t>
+  </si>
+  <si>
+    <t>blog.facebook.com</t>
+  </si>
+  <si>
+    <t>et-ee.facebook.com</t>
+  </si>
+  <si>
+    <t>nb-no.facebook.com</t>
+  </si>
+  <si>
+    <t>www.hs.facebook.com</t>
+  </si>
+  <si>
+    <t>rdg.facebook.com</t>
+  </si>
+  <si>
+    <t>www2.facebook.com</t>
+  </si>
+  <si>
+    <t>lists.facebook.com</t>
+  </si>
+  <si>
+    <t>ads.facebook.com</t>
+  </si>
+  <si>
+    <t>fa-ir.facebook.com</t>
+  </si>
+  <si>
+    <t>ro-ro.connect.facebook.com</t>
+  </si>
+  <si>
+    <t>fr-fr.facebook.com</t>
+  </si>
+  <si>
+    <t>www.facebook.com</t>
+  </si>
+  <si>
+    <t>www.k.connect.facebook.com</t>
+  </si>
+  <si>
+    <t>touch.facebook.com</t>
+  </si>
+  <si>
+    <t>es-la.f.connect.facebook.com</t>
+  </si>
+  <si>
+    <t>www.zh-cn.connect.facebook.com</t>
+  </si>
+  <si>
+    <t>fb-lt.facebook.com</t>
+  </si>
+  <si>
+    <t>fr-fr.o.facebook.com</t>
+  </si>
+  <si>
+    <t>ru-ru.facebook.com</t>
+  </si>
+  <si>
+    <t>nsa.facebook.com</t>
+  </si>
+  <si>
+    <t>pt-br.facebook.com</t>
+  </si>
+  <si>
+    <t>static.ak.facebook.com</t>
+  </si>
+  <si>
+    <t>cs-cz.facebook.com</t>
+  </si>
+  <si>
+    <t>pt-pt.facebook.com</t>
+  </si>
+  <si>
+    <t>abc.facebook.com</t>
+  </si>
+  <si>
+    <t>he-il.facebook.com</t>
+  </si>
+  <si>
+    <t>vi-vn.facebook.com</t>
+  </si>
+  <si>
+    <t>www.prod.facebook.com</t>
+  </si>
+  <si>
+    <t>postmaster.facebook.com</t>
+  </si>
+  <si>
+    <t>ww.facebook.com</t>
+  </si>
+  <si>
+    <t>bg-bg.facebook.com</t>
+  </si>
+  <si>
+    <t>ed.facebook.com</t>
+  </si>
+  <si>
+    <t>pacific.facebook.com</t>
+  </si>
+  <si>
+    <t>about.facebook.com</t>
+  </si>
+  <si>
+    <t>da-dk.facebook.com</t>
+  </si>
+  <si>
+    <t>sv-se.facebook.com</t>
+  </si>
+  <si>
+    <t>en-gb.facebook.com</t>
+  </si>
+  <si>
+    <t>nova.facebook.com</t>
+  </si>
+  <si>
+    <t>ko-kr.connect.facebook.com</t>
+  </si>
+  <si>
+    <t>ns3.facebook.com</t>
+  </si>
+  <si>
+    <t>de-de.facebook.com</t>
+  </si>
+  <si>
+    <t>nl-nl.facebook.com</t>
+  </si>
+  <si>
+    <t>upload.facebook.com</t>
+  </si>
+  <si>
+    <t>apps.facebook.com</t>
+  </si>
+  <si>
+    <t>zh-hk.facebook.com</t>
+  </si>
+  <si>
+    <t>ar-ar.vn-ni.connect.facebook.com</t>
+  </si>
+  <si>
+    <t>v4help.facebook.com</t>
+  </si>
+  <si>
+    <t>national.facebook.com</t>
+  </si>
+  <si>
+    <t>mbasic.facebook.com</t>
+  </si>
+  <si>
+    <t>it-it.facebook.com</t>
+  </si>
+  <si>
+    <t>ro-ro.facebook.com</t>
+  </si>
+  <si>
+    <t>fr.facebook.com</t>
+  </si>
+  <si>
+    <t>ns1.facebook.com</t>
+  </si>
+  <si>
+    <t>nl.facebook.com</t>
+  </si>
+  <si>
+    <t>beta.facebook.com</t>
+  </si>
+  <si>
+    <t>zh-cn.facebook.com</t>
+  </si>
+  <si>
+    <t>wwww.facebook.com</t>
+  </si>
+  <si>
+    <t>c.facebook.com</t>
+  </si>
+  <si>
+    <t>0.facebook.com</t>
+  </si>
+  <si>
+    <t>tr-tr.facebook.com</t>
+  </si>
+  <si>
+    <t>Register.facebook.com</t>
+  </si>
+  <si>
+    <t>Fr-ca.facebook.com</t>
+  </si>
+  <si>
+    <t>Es-es.facebook.com</t>
+  </si>
+  <si>
+    <t>Ko-kr.facebook.com</t>
+  </si>
+  <si>
+    <t>iPhone.facebook.com</t>
+  </si>
+  <si>
+    <t>d.facebook.com</t>
+  </si>
+  <si>
+    <t>m.facebook.com</t>
+  </si>
+  <si>
+    <t>hr-hr.facebook.com</t>
+  </si>
+  <si>
+    <t>it.facebook.com</t>
+  </si>
+  <si>
+    <t>bs-ba.facebook.com</t>
+  </si>
+  <si>
+    <t>vi-vn.o.facebook.com</t>
+  </si>
+  <si>
+    <t>ms-my.facebook.com</t>
+  </si>
+  <si>
+    <t>Secure.facebook.com</t>
+  </si>
+  <si>
+    <t>Pixel.facebook.com</t>
+  </si>
+  <si>
+    <t>Sr-rs.facebook.com</t>
+  </si>
+  <si>
+    <t>H.facebook.com</t>
+  </si>
+  <si>
+    <t>Hu-hu.facebook.com</t>
+  </si>
+  <si>
+    <t>Pl-pl.facebook.com</t>
+  </si>
+  <si>
+    <t>Badge.facebook.com</t>
+  </si>
+  <si>
+    <t>Accounts.fb.com</t>
+  </si>
+  <si>
+    <t>Investor.fb.com</t>
+  </si>
+  <si>
+    <t>Files.fb.com</t>
+  </si>
+  <si>
+    <t>Vsp.fb.com</t>
+  </si>
+  <si>
+    <t>S.fb.com</t>
+  </si>
+  <si>
+    <t>Docs.fb.com</t>
+  </si>
+  <si>
+    <t>Newsroom.fb.com</t>
+  </si>
+  <si>
+    <t>Search.fb.com</t>
+  </si>
+  <si>
+    <t>www.fb.com</t>
+  </si>
+  <si>
+    <t>www.beta.facebook.com</t>
+  </si>
+  <si>
+    <t>www.connect.facebook.com</t>
+  </si>
+  <si>
+    <t>www.ebuddy.com.php.zero.facebook.com</t>
   </si>
 </sst>
 </file>
@@ -4826,10 +5186,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1269"/>
+  <dimension ref="A1:B1389"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A1379" workbookViewId="0">
+      <selection activeCell="A1269" sqref="A1269:A1389"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14984,6 +15344,966 @@
       </c>
       <c r="B1269" t="s">
         <v>1268</v>
+      </c>
+    </row>
+    <row r="1270" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1270" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1270" t="s">
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="1271" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1271" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1271" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="1272" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1272" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1272" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="1273" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1273" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1273" t="s">
+        <v>1324</v>
+      </c>
+    </row>
+    <row r="1274" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1274" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1274" t="s">
+        <v>1325</v>
+      </c>
+    </row>
+    <row r="1275" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1275" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1275" t="s">
+        <v>1326</v>
+      </c>
+    </row>
+    <row r="1276" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1276" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1276" t="s">
+        <v>1327</v>
+      </c>
+    </row>
+    <row r="1277" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1277" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1277" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="1278" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1278" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1278" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="1279" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1279" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1279" t="s">
+        <v>1330</v>
+      </c>
+    </row>
+    <row r="1280" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1280" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1280" t="s">
+        <v>1331</v>
+      </c>
+    </row>
+    <row r="1281" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1281" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1281" t="s">
+        <v>1332</v>
+      </c>
+    </row>
+    <row r="1282" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1282" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1282" t="s">
+        <v>1333</v>
+      </c>
+    </row>
+    <row r="1283" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1283" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1283" t="s">
+        <v>1334</v>
+      </c>
+    </row>
+    <row r="1284" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1284" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1284" t="s">
+        <v>1335</v>
+      </c>
+    </row>
+    <row r="1285" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1285" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1285" t="s">
+        <v>1336</v>
+      </c>
+    </row>
+    <row r="1286" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1286" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1286" t="s">
+        <v>1337</v>
+      </c>
+    </row>
+    <row r="1287" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1287" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1287" t="s">
+        <v>1338</v>
+      </c>
+    </row>
+    <row r="1288" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1288" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1288" t="s">
+        <v>1339</v>
+      </c>
+    </row>
+    <row r="1289" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1289" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1289" t="s">
+        <v>1340</v>
+      </c>
+    </row>
+    <row r="1290" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1290" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1290" t="s">
+        <v>1341</v>
+      </c>
+    </row>
+    <row r="1291" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1291" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1291" t="s">
+        <v>1342</v>
+      </c>
+    </row>
+    <row r="1292" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1292" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1292" t="s">
+        <v>1343</v>
+      </c>
+    </row>
+    <row r="1293" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1293" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1293" t="s">
+        <v>1344</v>
+      </c>
+    </row>
+    <row r="1294" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1294" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1294" t="s">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="1295" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1295" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1295" t="s">
+        <v>1346</v>
+      </c>
+    </row>
+    <row r="1296" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1296" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1296" t="s">
+        <v>1347</v>
+      </c>
+    </row>
+    <row r="1297" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1297" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1297" t="s">
+        <v>1348</v>
+      </c>
+    </row>
+    <row r="1298" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1298" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1298" t="s">
+        <v>1349</v>
+      </c>
+    </row>
+    <row r="1299" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1299" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1299" t="s">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="1300" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1300" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1300" t="s">
+        <v>1351</v>
+      </c>
+    </row>
+    <row r="1301" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1301" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1301" t="s">
+        <v>1352</v>
+      </c>
+    </row>
+    <row r="1302" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1302" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1302" t="s">
+        <v>1353</v>
+      </c>
+    </row>
+    <row r="1303" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1303" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1303" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="1304" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1304" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1304" t="s">
+        <v>1355</v>
+      </c>
+    </row>
+    <row r="1305" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1305" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1305" t="s">
+        <v>1356</v>
+      </c>
+    </row>
+    <row r="1306" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1306" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1306" t="s">
+        <v>1357</v>
+      </c>
+    </row>
+    <row r="1307" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1307" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1307" t="s">
+        <v>1358</v>
+      </c>
+    </row>
+    <row r="1308" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1308" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1308" t="s">
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="1309" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1309" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1309" t="s">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="1310" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1310" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1310" t="s">
+        <v>1361</v>
+      </c>
+    </row>
+    <row r="1311" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1311" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1311" t="s">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="1312" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1312" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1312" t="s">
+        <v>1363</v>
+      </c>
+    </row>
+    <row r="1313" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1313" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1313" t="s">
+        <v>1364</v>
+      </c>
+    </row>
+    <row r="1314" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1314" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1314" t="s">
+        <v>1365</v>
+      </c>
+    </row>
+    <row r="1315" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1315" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1315" t="s">
+        <v>1366</v>
+      </c>
+    </row>
+    <row r="1316" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1316" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1316" t="s">
+        <v>1367</v>
+      </c>
+    </row>
+    <row r="1317" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1317" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1317" t="s">
+        <v>1368</v>
+      </c>
+    </row>
+    <row r="1318" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1318" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1318" t="s">
+        <v>1369</v>
+      </c>
+    </row>
+    <row r="1319" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1319" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1319" t="s">
+        <v>1370</v>
+      </c>
+    </row>
+    <row r="1320" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1320" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1320" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="1321" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1321" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1321" t="s">
+        <v>1372</v>
+      </c>
+    </row>
+    <row r="1322" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1322" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1322" t="s">
+        <v>1373</v>
+      </c>
+    </row>
+    <row r="1323" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1323" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1323" t="s">
+        <v>1374</v>
+      </c>
+    </row>
+    <row r="1324" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1324" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1324" t="s">
+        <v>1375</v>
+      </c>
+    </row>
+    <row r="1325" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1325" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1325" t="s">
+        <v>1376</v>
+      </c>
+    </row>
+    <row r="1326" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1326" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1326" t="s">
+        <v>1377</v>
+      </c>
+    </row>
+    <row r="1327" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1327" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1327" t="s">
+        <v>1378</v>
+      </c>
+    </row>
+    <row r="1328" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1328" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1328" t="s">
+        <v>1379</v>
+      </c>
+    </row>
+    <row r="1329" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1329" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1329" t="s">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="1330" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1330" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1330" t="s">
+        <v>1381</v>
+      </c>
+    </row>
+    <row r="1331" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1331" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1331" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="1332" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1332" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1332" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="1333" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1333" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1333" t="s">
+        <v>1384</v>
+      </c>
+    </row>
+    <row r="1334" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1334" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1334" t="s">
+        <v>1385</v>
+      </c>
+    </row>
+    <row r="1335" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1335" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1335" t="s">
+        <v>1386</v>
+      </c>
+    </row>
+    <row r="1336" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1336" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1336" t="s">
+        <v>1387</v>
+      </c>
+    </row>
+    <row r="1337" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1337" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1337" t="s">
+        <v>1388</v>
+      </c>
+    </row>
+    <row r="1338" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1338" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1338" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="1339" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1339" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1339" t="s">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="1340" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1340" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1340" t="s">
+        <v>1391</v>
+      </c>
+    </row>
+    <row r="1341" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1341" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1341" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="1342" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1342" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1342" t="s">
+        <v>1393</v>
+      </c>
+    </row>
+    <row r="1343" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1343" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1343" t="s">
+        <v>1394</v>
+      </c>
+    </row>
+    <row r="1344" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1344" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1344" t="s">
+        <v>1395</v>
+      </c>
+    </row>
+    <row r="1345" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1345" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1345" t="s">
+        <v>1396</v>
+      </c>
+    </row>
+    <row r="1346" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1346" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1346" t="s">
+        <v>1397</v>
+      </c>
+    </row>
+    <row r="1347" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1347" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1347" t="s">
+        <v>1398</v>
+      </c>
+    </row>
+    <row r="1348" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1348" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1348" t="s">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="1349" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1349" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1349" t="s">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="1350" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1350" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1350" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="1351" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1351" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1351" t="s">
+        <v>1402</v>
+      </c>
+    </row>
+    <row r="1352" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1352" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1352" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="1353" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1353" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1353" t="s">
+        <v>1404</v>
+      </c>
+    </row>
+    <row r="1354" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1354" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1354" t="s">
+        <v>1405</v>
+      </c>
+    </row>
+    <row r="1355" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1355" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1355" t="s">
+        <v>1406</v>
+      </c>
+    </row>
+    <row r="1356" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1356" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1356" t="s">
+        <v>1407</v>
+      </c>
+    </row>
+    <row r="1357" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1357" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1357" t="s">
+        <v>1408</v>
+      </c>
+    </row>
+    <row r="1358" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1358" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1358" t="s">
+        <v>1409</v>
+      </c>
+    </row>
+    <row r="1359" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1359" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1359" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="1360" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1360" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1360" t="s">
+        <v>1411</v>
+      </c>
+    </row>
+    <row r="1361" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1361" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1361" t="s">
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="1362" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1362" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1362" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="1363" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1363" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1363" t="s">
+        <v>1414</v>
+      </c>
+    </row>
+    <row r="1364" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1364" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1364" t="s">
+        <v>1415</v>
+      </c>
+    </row>
+    <row r="1365" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1365" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1365" t="s">
+        <v>1416</v>
+      </c>
+    </row>
+    <row r="1366" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1366" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1366" t="s">
+        <v>1417</v>
+      </c>
+    </row>
+    <row r="1367" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1367" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1367" t="s">
+        <v>1418</v>
+      </c>
+    </row>
+    <row r="1368" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1368" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1368" t="s">
+        <v>1419</v>
+      </c>
+    </row>
+    <row r="1369" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1369" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1369" t="s">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="1370" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1370" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1370" t="s">
+        <v>1421</v>
+      </c>
+    </row>
+    <row r="1371" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1371" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1371" t="s">
+        <v>1422</v>
+      </c>
+    </row>
+    <row r="1372" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1372" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1372" t="s">
+        <v>1423</v>
+      </c>
+    </row>
+    <row r="1373" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1373" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1373" t="s">
+        <v>1424</v>
+      </c>
+    </row>
+    <row r="1374" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1374" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1374" t="s">
+        <v>1425</v>
+      </c>
+    </row>
+    <row r="1375" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1375" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1375" t="s">
+        <v>1426</v>
+      </c>
+    </row>
+    <row r="1376" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1376" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1376" t="s">
+        <v>1427</v>
+      </c>
+    </row>
+    <row r="1377" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1377" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1377" t="s">
+        <v>1428</v>
+      </c>
+    </row>
+    <row r="1378" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1378" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1378" t="s">
+        <v>1429</v>
+      </c>
+    </row>
+    <row r="1379" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1379" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1379" t="s">
+        <v>1430</v>
+      </c>
+    </row>
+    <row r="1380" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1380" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1380" t="s">
+        <v>1431</v>
+      </c>
+    </row>
+    <row r="1381" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1381" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1381" t="s">
+        <v>1432</v>
+      </c>
+    </row>
+    <row r="1382" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1382" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1382" t="s">
+        <v>1433</v>
+      </c>
+    </row>
+    <row r="1383" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1383" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1383" t="s">
+        <v>1434</v>
+      </c>
+    </row>
+    <row r="1384" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1384" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1384" t="s">
+        <v>1435</v>
+      </c>
+    </row>
+    <row r="1385" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1385" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1385" t="s">
+        <v>1436</v>
+      </c>
+    </row>
+    <row r="1386" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1386" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1386" t="s">
+        <v>1437</v>
+      </c>
+    </row>
+    <row r="1387" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1387" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1387" t="s">
+        <v>1438</v>
+      </c>
+    </row>
+    <row r="1388" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1388" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1388" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="1389" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1389" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1389" t="s">
+        <v>1440</v>
       </c>
     </row>
   </sheetData>
@@ -14995,7 +16315,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1449AAE8-39C4-4456-952F-441D8B4FD7B4}">
   <dimension ref="A1:B1311"/>
   <sheetViews>
-    <sheetView topLeftCell="A1273" workbookViewId="0">
+    <sheetView topLeftCell="A1339" workbookViewId="0">
       <selection sqref="A1:B1311"/>
     </sheetView>
   </sheetViews>
@@ -25501,7 +26821,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1619F29A-E844-45C8-9B69-B2FC52131404}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1642" workbookViewId="0">
+    <sheetView topLeftCell="A1642" workbookViewId="0">
       <selection activeCell="F1649" sqref="F1649"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Adding Tik Tok because of course I am
</commit_message>
<xml_diff>
--- a/blocklist work in process.xlsx
+++ b/blocklist work in process.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brian\Documents\Git Projects\Ad List\adlist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED335038-2F96-436D-AEFD-C733D554C0FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33B9E234-EDB7-4917-AF01-A6758A6BEF31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="1140" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5400" uniqueCount="1441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5514" uniqueCount="1476">
   <si>
     <t>api-v3.tinypass.com</t>
   </si>
@@ -4345,6 +4345,111 @@
   </si>
   <si>
     <t>www.ebuddy.com.php.zero.facebook.com</t>
+  </si>
+  <si>
+    <t>v16a.tiktokcdn.com</t>
+  </si>
+  <si>
+    <t>p16-tiktokcdn-com.akamaized.net</t>
+  </si>
+  <si>
+    <t>log.tiktokv.com</t>
+  </si>
+  <si>
+    <t>ib.tiktokv.com</t>
+  </si>
+  <si>
+    <t>api-h2.tiktokv.com</t>
+  </si>
+  <si>
+    <t>v16m.tiktokcdn.com</t>
+  </si>
+  <si>
+    <t>api.tiktokv.com</t>
+  </si>
+  <si>
+    <t>v19.tiktokcdn.com</t>
+  </si>
+  <si>
+    <t>mon.musical.ly</t>
+  </si>
+  <si>
+    <t>api2-16-h2.musical.ly</t>
+  </si>
+  <si>
+    <t>api2.musical.ly</t>
+  </si>
+  <si>
+    <t>log2.musical.ly</t>
+  </si>
+  <si>
+    <t>api2-21-h2.musical.ly</t>
+  </si>
+  <si>
+    <t>api21-h2.tiktokv.com</t>
+  </si>
+  <si>
+    <t>m.tiktok.com</t>
+  </si>
+  <si>
+    <t>muscdn.com</t>
+  </si>
+  <si>
+    <t>tiktokcdn.com</t>
+  </si>
+  <si>
+    <t>tiktokcdn.com.c.worldfcdn.com</t>
+  </si>
+  <si>
+    <t>*.tiktok.com</t>
+  </si>
+  <si>
+    <t>www.tiktok.com</t>
+  </si>
+  <si>
+    <t>ns-440.awsdns-55.com</t>
+  </si>
+  <si>
+    <t>ns-722.awsdns-26.net</t>
+  </si>
+  <si>
+    <t>ns-1475.awsdns-56.org</t>
+  </si>
+  <si>
+    <t>ns-1574.awsdns-04.co.uk</t>
+  </si>
+  <si>
+    <t>tiktokcdn-com.akamaized.net</t>
+  </si>
+  <si>
+    <t>t.tiktok.com</t>
+  </si>
+  <si>
+    <t>tiktok.org</t>
+  </si>
+  <si>
+    <t>tiktokv.com</t>
+  </si>
+  <si>
+    <t>vt.tiktok.com</t>
+  </si>
+  <si>
+    <t>v16.tiktokcdn.com</t>
+  </si>
+  <si>
+    <t>mon.tiktokv.com</t>
+  </si>
+  <si>
+    <t>v16-tiktokcdn-com.akamaized.net</t>
+  </si>
+  <si>
+    <t>musical.ly</t>
+  </si>
+  <si>
+    <t>akamai.net</t>
+  </si>
+  <si>
+    <t>isnssdk.com</t>
   </si>
 </sst>
 </file>
@@ -5186,10 +5291,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1389"/>
+  <dimension ref="A1:B1446"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1379" workbookViewId="0">
-      <selection activeCell="A1269" sqref="A1269:A1389"/>
+    <sheetView tabSelected="1" topLeftCell="A1361" workbookViewId="0">
+      <selection activeCell="A1389" sqref="A1389:A1446"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16304,6 +16409,462 @@
       </c>
       <c r="B1389" t="s">
         <v>1440</v>
+      </c>
+    </row>
+    <row r="1390" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1390" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1390" t="s">
+        <v>1441</v>
+      </c>
+    </row>
+    <row r="1391" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1391" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1391" t="s">
+        <v>1442</v>
+      </c>
+    </row>
+    <row r="1392" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1392" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1392" t="s">
+        <v>1443</v>
+      </c>
+    </row>
+    <row r="1393" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1393" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1393" t="s">
+        <v>1444</v>
+      </c>
+    </row>
+    <row r="1394" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1394" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1394" t="s">
+        <v>1445</v>
+      </c>
+    </row>
+    <row r="1395" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1395" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1395" t="s">
+        <v>1446</v>
+      </c>
+    </row>
+    <row r="1396" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1396" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1396" t="s">
+        <v>1447</v>
+      </c>
+    </row>
+    <row r="1397" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1397" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1397" t="s">
+        <v>1448</v>
+      </c>
+    </row>
+    <row r="1398" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1398" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1398" t="s">
+        <v>1449</v>
+      </c>
+    </row>
+    <row r="1399" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1399" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1399" t="s">
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="1400" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1400" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1400" t="s">
+        <v>1451</v>
+      </c>
+    </row>
+    <row r="1401" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1401" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1401" t="s">
+        <v>1452</v>
+      </c>
+    </row>
+    <row r="1402" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1402" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1402" t="s">
+        <v>1453</v>
+      </c>
+    </row>
+    <row r="1403" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1403" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1403" t="s">
+        <v>1445</v>
+      </c>
+    </row>
+    <row r="1404" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1404" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1404" t="s">
+        <v>1447</v>
+      </c>
+    </row>
+    <row r="1405" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1405" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1405" t="s">
+        <v>1454</v>
+      </c>
+    </row>
+    <row r="1406" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1406" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1406" t="s">
+        <v>1444</v>
+      </c>
+    </row>
+    <row r="1407" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1407" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1407" t="s">
+        <v>1455</v>
+      </c>
+    </row>
+    <row r="1408" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1408" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1408" t="s">
+        <v>1456</v>
+      </c>
+    </row>
+    <row r="1409" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1409" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1409" t="s">
+        <v>1457</v>
+      </c>
+    </row>
+    <row r="1410" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1410" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1410" t="s">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="1411" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1411" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1411" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="1412" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1412" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1412" t="s">
+        <v>1459</v>
+      </c>
+    </row>
+    <row r="1413" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1413" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1413" t="s">
+        <v>1460</v>
+      </c>
+    </row>
+    <row r="1414" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1414" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1414" t="s">
+        <v>1445</v>
+      </c>
+    </row>
+    <row r="1415" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1415" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1415" t="s">
+        <v>1454</v>
+      </c>
+    </row>
+    <row r="1416" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1416" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1416" t="s">
+        <v>1461</v>
+      </c>
+    </row>
+    <row r="1417" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1417" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1417" t="s">
+        <v>1462</v>
+      </c>
+    </row>
+    <row r="1418" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1418" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1418" t="s">
+        <v>1463</v>
+      </c>
+    </row>
+    <row r="1419" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1419" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1419" t="s">
+        <v>1464</v>
+      </c>
+    </row>
+    <row r="1420" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1420" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1420" t="s">
+        <v>1465</v>
+      </c>
+    </row>
+    <row r="1421" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1421" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1421" t="s">
+        <v>1445</v>
+      </c>
+    </row>
+    <row r="1422" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1422" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1422" t="s">
+        <v>1454</v>
+      </c>
+    </row>
+    <row r="1423" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1423" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1423" t="s">
+        <v>1461</v>
+      </c>
+    </row>
+    <row r="1424" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1424" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1424" t="s">
+        <v>1462</v>
+      </c>
+    </row>
+    <row r="1425" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1425" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1425" t="s">
+        <v>1463</v>
+      </c>
+    </row>
+    <row r="1426" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1426" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1426" t="s">
+        <v>1464</v>
+      </c>
+    </row>
+    <row r="1427" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1427" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1427" t="s">
+        <v>1465</v>
+      </c>
+    </row>
+    <row r="1428" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1428" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1428" t="s">
+        <v>1455</v>
+      </c>
+    </row>
+    <row r="1429" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1429" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1429" t="s">
+        <v>1466</v>
+      </c>
+    </row>
+    <row r="1430" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1430" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1430" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="1431" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1431" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1431" t="s">
+        <v>1467</v>
+      </c>
+    </row>
+    <row r="1432" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1432" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1432" t="s">
+        <v>1457</v>
+      </c>
+    </row>
+    <row r="1433" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1433" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1433" t="s">
+        <v>1468</v>
+      </c>
+    </row>
+    <row r="1434" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1434" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1434" t="s">
+        <v>1469</v>
+      </c>
+    </row>
+    <row r="1435" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1435" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1435" t="s">
+        <v>1448</v>
+      </c>
+    </row>
+    <row r="1436" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1436" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1436" t="s">
+        <v>1470</v>
+      </c>
+    </row>
+    <row r="1437" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1437" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1437" t="s">
+        <v>1447</v>
+      </c>
+    </row>
+    <row r="1438" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1438" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1438" t="s">
+        <v>1471</v>
+      </c>
+    </row>
+    <row r="1439" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1439" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1439" t="s">
+        <v>1444</v>
+      </c>
+    </row>
+    <row r="1440" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1440" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1440" t="s">
+        <v>1442</v>
+      </c>
+    </row>
+    <row r="1441" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1441" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1441" t="s">
+        <v>1472</v>
+      </c>
+    </row>
+    <row r="1442" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1442" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1442" t="s">
+        <v>1473</v>
+      </c>
+    </row>
+    <row r="1443" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1443" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1443" t="s">
+        <v>1456</v>
+      </c>
+    </row>
+    <row r="1444" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1444" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1444" t="s">
+        <v>1474</v>
+      </c>
+    </row>
+    <row r="1445" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1445" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1445" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="1446" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1446" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1446" t="s">
+        <v>1460</v>
       </c>
     </row>
   </sheetData>

</xml_diff>